<commit_message>
june 23 (before ICC removal)
</commit_message>
<xml_diff>
--- a/Reports/Lobewise Comparisons/ResultsFinal/atel.xlsx
+++ b/Reports/Lobewise Comparisons/ResultsFinal/atel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c2d16a148962151/Desktop/BIOSTAT/Thesis/Thesis/Reports/Lobewise Comparisons/ResultsFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC1048CA799F592E5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D9B7A7-9E83-4119-81DA-F576B01C4D56}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC1048CA799F592E5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75560A1-399A-49A8-9DF7-D70FE39A4A5F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO_main" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>LLL vs LUS</t>
   </si>
   <si>
-    <t>LUS vs RUL</t>
+    <t>LUS vs RLL</t>
   </si>
 </sst>
 </file>
@@ -137,9 +137,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +154,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,7 +426,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -504,7 +507,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -530,7 +533,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -556,7 +559,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -579,7 +582,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
@@ -602,7 +605,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -628,7 +631,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -654,7 +657,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -677,7 +680,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -700,7 +703,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -723,7 +726,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13">
@@ -749,7 +752,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14">
@@ -775,7 +778,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15">
@@ -798,7 +801,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16">

</xml_diff>